<commit_message>
June 28, try to break transition path into 4 functions
</commit_message>
<xml_diff>
--- a/twoplaneproblem.xlsx
+++ b/twoplaneproblem.xlsx
@@ -502,11 +502,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2080611192"/>
-        <c:axId val="2081778664"/>
+        <c:axId val="2117612888"/>
+        <c:axId val="2116726728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2080611192"/>
+        <c:axId val="2117612888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -515,7 +515,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2081778664"/>
+        <c:crossAx val="2116726728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -523,7 +523,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2081778664"/>
+        <c:axId val="2116726728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -534,14 +534,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2080611192"/>
+        <c:crossAx val="2117612888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -862,11 +861,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2133404232"/>
-        <c:axId val="2133748056"/>
+        <c:axId val="2117680920"/>
+        <c:axId val="2117683896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2133404232"/>
+        <c:axId val="2117680920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -875,7 +874,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2133748056"/>
+        <c:crossAx val="2117683896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -883,7 +882,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2133748056"/>
+        <c:axId val="2117683896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -894,14 +893,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2133404232"/>
+        <c:crossAx val="2117680920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2341,7 +2339,6 @@
     <mergeCell ref="C3:I3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5430,7 +5427,6 @@
     <mergeCell ref="C3:I3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>